<commit_message>
cambios en cus 7
</commit_message>
<xml_diff>
--- a/analisis/casos_de_usos/CUS-007 Realizar una reserva.xlsx
+++ b/analisis/casos_de_usos/CUS-007 Realizar una reserva.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\Desktop\ratos\casos_de_uso\appp\analisis\casos_de_usos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5959CFA2-9831-4466-81C8-F5FEF480A388}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2BC2E25-415C-4FED-8FCD-6CF2EE74ADCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="1245" windowWidth="16800" windowHeight="13425" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1830" yWindow="1695" windowWidth="16800" windowHeight="13425" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CASO DE USO" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
   <si>
     <t>ID CASO DE USO</t>
   </si>
@@ -85,19 +85,37 @@
     <t>Flujo Alternativo 2:</t>
   </si>
   <si>
-    <t>Flujo Alternativo 1:</t>
-  </si>
-  <si>
     <t>Permite a un cliente realizar su reserva.</t>
-  </si>
-  <si>
-    <t>tener sesion iniciada</t>
   </si>
   <si>
     <t>Consultar cancha</t>
   </si>
   <si>
     <t>Reserva activa y registrada</t>
+  </si>
+  <si>
+    <t>El cliente debe estar autenticado.</t>
+  </si>
+  <si>
+    <t>El cliente debe darle a la opcion "hacer reserva"</t>
+  </si>
+  <si>
+    <t>Elegir la hora a reservar de las opciones proporcionadas</t>
+  </si>
+  <si>
+    <t>elegir el dia a reservar</t>
+  </si>
+  <si>
+    <t>Ese dia ya se encuentra reservado</t>
+  </si>
+  <si>
+    <t>Se enviara un mensaje de error "este dia y hora ya esta reservada".</t>
+  </si>
+  <si>
+    <t>Flujo Alternativo 1: reservas</t>
+  </si>
+  <si>
+    <t>Mostrar un mensaje "la reserva a sido exitosa"</t>
   </si>
 </sst>
 </file>
@@ -618,6 +636,10 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -628,6 +650,12 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -638,16 +666,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -869,9 +887,9 @@
   </sheetPr>
   <dimension ref="A1:V987"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D20" sqref="D20"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C29" sqref="C29:E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -938,7 +956,7 @@
     <row r="3" spans="1:22" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
-      <c r="C3" s="48" t="s">
+      <c r="C3" s="36" t="s">
         <v>13</v>
       </c>
       <c r="D3" s="7"/>
@@ -992,10 +1010,10 @@
     <row r="5" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
       <c r="B5" s="9"/>
-      <c r="C5" s="48" t="s">
+      <c r="C5" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="48" t="s">
+      <c r="D5" s="36" t="s">
         <v>15</v>
       </c>
       <c r="E5" s="5"/>
@@ -1146,10 +1164,10 @@
     <row r="11" spans="1:22" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
-      <c r="C11" s="49" t="s">
-        <v>18</v>
+      <c r="C11" s="44" t="s">
+        <v>17</v>
       </c>
-      <c r="D11" s="50"/>
+      <c r="D11" s="45"/>
       <c r="E11" s="5"/>
       <c r="F11" s="8"/>
       <c r="G11" s="8"/>
@@ -1276,8 +1294,8 @@
       <c r="B16" s="19">
         <v>1</v>
       </c>
-      <c r="C16" s="51" t="s">
-        <v>19</v>
+      <c r="C16" s="37" t="s">
+        <v>20</v>
       </c>
       <c r="D16" s="13"/>
       <c r="E16" s="13"/>
@@ -1304,8 +1322,8 @@
       <c r="B17" s="21">
         <v>2</v>
       </c>
-      <c r="C17" s="51" t="s">
-        <v>20</v>
+      <c r="C17" s="37" t="s">
+        <v>18</v>
       </c>
       <c r="D17" s="13"/>
       <c r="E17" s="13"/>
@@ -1384,8 +1402,8 @@
       <c r="B20" s="19">
         <v>1</v>
       </c>
-      <c r="C20" s="51" t="s">
-        <v>21</v>
+      <c r="C20" s="37" t="s">
+        <v>19</v>
       </c>
       <c r="D20" s="13"/>
       <c r="E20" s="13"/>
@@ -1486,11 +1504,11 @@
       <c r="B24" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C24" s="42" t="s">
+      <c r="C24" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="D24" s="43"/>
-      <c r="E24" s="44"/>
+      <c r="D24" s="47"/>
+      <c r="E24" s="48"/>
       <c r="F24" s="8"/>
       <c r="G24" s="8"/>
       <c r="H24" s="8"/>
@@ -1540,9 +1558,11 @@
       <c r="B26" s="19">
         <v>1</v>
       </c>
-      <c r="C26" s="45"/>
-      <c r="D26" s="46"/>
-      <c r="E26" s="47"/>
+      <c r="C26" s="49" t="s">
+        <v>21</v>
+      </c>
+      <c r="D26" s="50"/>
+      <c r="E26" s="51"/>
       <c r="F26" s="8"/>
       <c r="G26" s="8"/>
       <c r="H26" s="8"/>
@@ -1566,9 +1586,11 @@
       <c r="B27" s="26">
         <v>2</v>
       </c>
-      <c r="C27" s="39"/>
-      <c r="D27" s="40"/>
-      <c r="E27" s="41"/>
+      <c r="C27" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="D27" s="42"/>
+      <c r="E27" s="43"/>
       <c r="F27" s="8"/>
       <c r="G27" s="8"/>
       <c r="H27" s="8"/>
@@ -1592,9 +1614,11 @@
       <c r="B28" s="26">
         <v>3</v>
       </c>
-      <c r="C28" s="39"/>
-      <c r="D28" s="40"/>
-      <c r="E28" s="41"/>
+      <c r="C28" s="41" t="s">
+        <v>23</v>
+      </c>
+      <c r="D28" s="42"/>
+      <c r="E28" s="43"/>
       <c r="F28" s="8"/>
       <c r="G28" s="8"/>
       <c r="H28" s="8"/>
@@ -1618,9 +1642,11 @@
       <c r="B29" s="26">
         <v>4</v>
       </c>
-      <c r="C29" s="39"/>
-      <c r="D29" s="40"/>
-      <c r="E29" s="41"/>
+      <c r="C29" s="41" t="s">
+        <v>27</v>
+      </c>
+      <c r="D29" s="42"/>
+      <c r="E29" s="43"/>
       <c r="F29" s="8"/>
       <c r="G29" s="8"/>
       <c r="H29" s="8"/>
@@ -1642,7 +1668,7 @@
     <row r="30" spans="1:22" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="24"/>
       <c r="B30" s="17" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="C30" s="27"/>
       <c r="D30" s="25"/>
@@ -1670,9 +1696,11 @@
       <c r="B31" s="21">
         <v>5</v>
       </c>
-      <c r="C31" s="39"/>
-      <c r="D31" s="40"/>
-      <c r="E31" s="41"/>
+      <c r="C31" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="D31" s="42"/>
+      <c r="E31" s="43"/>
       <c r="F31" s="8"/>
       <c r="G31" s="8"/>
       <c r="H31" s="8"/>
@@ -1696,9 +1724,11 @@
       <c r="B32" s="28">
         <v>6</v>
       </c>
-      <c r="C32" s="36"/>
-      <c r="D32" s="37"/>
-      <c r="E32" s="38"/>
+      <c r="C32" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="D32" s="39"/>
+      <c r="E32" s="40"/>
       <c r="F32" s="8"/>
       <c r="G32" s="8"/>
       <c r="H32" s="8"/>
@@ -1748,9 +1778,9 @@
       <c r="B34" s="28">
         <v>7</v>
       </c>
-      <c r="C34" s="39"/>
-      <c r="D34" s="40"/>
-      <c r="E34" s="41"/>
+      <c r="C34" s="41"/>
+      <c r="D34" s="42"/>
+      <c r="E34" s="43"/>
       <c r="F34" s="8"/>
       <c r="G34" s="8"/>
       <c r="H34" s="8"/>
@@ -1774,9 +1804,9 @@
       <c r="B35" s="28">
         <v>8</v>
       </c>
-      <c r="C35" s="39"/>
-      <c r="D35" s="40"/>
-      <c r="E35" s="41"/>
+      <c r="C35" s="41"/>
+      <c r="D35" s="42"/>
+      <c r="E35" s="43"/>
       <c r="F35" s="8"/>
       <c r="G35" s="8"/>
       <c r="H35" s="8"/>

</xml_diff>